<commit_message>
Daily tasks solving and fix
</commit_message>
<xml_diff>
--- a/Interview preposition 2019.xlsx
+++ b/Interview preposition 2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\YandexDisk\Interview Prep 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775975AD-2CD6-4E3C-B2D9-ACCE7F528BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72871D8F-6A81-4C9A-865C-C660A56D2717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="2535" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="2640" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="286">
   <si>
     <t>Number</t>
   </si>
@@ -877,6 +877,9 @@
   </si>
   <si>
     <t>Pairs of Songs With Total Durations Divisible by 60</t>
+  </si>
+  <si>
+    <t>The K Weakest Rows in a Matrix</t>
   </si>
 </sst>
 </file>
@@ -1417,10 +1420,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="F252" sqref="F252"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="F251" sqref="F251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7205,6 +7208,29 @@
       </c>
       <c r="G251" s="19">
         <v>43861</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>1341</v>
+      </c>
+      <c r="B252" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="C252" t="s">
+        <v>15</v>
+      </c>
+      <c r="D252" t="s">
+        <v>12</v>
+      </c>
+      <c r="E252" t="s">
+        <v>11</v>
+      </c>
+      <c r="F252" t="s">
+        <v>8</v>
+      </c>
+      <c r="G252" s="19">
+        <v>43864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>